<commit_message>
New temperature sensor + stabilizations delays in HV init
Added functions to interface with the new type of temperature sensors +
added to register
Added 1.5s delay before checking the 2.5V feedback from the HV supplies
to wait for it to stabilize (not enabled yet)
Deactivated the electrode actuation loop
</commit_message>
<xml_diff>
--- a/FunctionStatus.xlsx
+++ b/FunctionStatus.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="100">
   <si>
     <t>File</t>
   </si>
@@ -149,9 +149,6 @@
     <t>SendFeedback</t>
   </si>
   <si>
-    <t>Test with Checksum</t>
-  </si>
-  <si>
     <t>POWER_INIT</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>NOT WORKING</t>
-  </si>
-  <si>
     <t>SEP_DEV_INIT</t>
   </si>
   <si>
@@ -251,9 +245,6 @@
     <t>Algorithms.h</t>
   </si>
   <si>
-    <t>SetMode</t>
-  </si>
-  <si>
     <t>Under construction</t>
   </si>
   <si>
@@ -330,6 +321,9 @@
   </si>
   <si>
     <t>TESTED</t>
+  </si>
+  <si>
+    <t>Work for board sensors. Need to test IR sensors</t>
   </si>
 </sst>
 </file>
@@ -663,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,7 +687,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>8</v>
@@ -710,10 +704,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="1">
         <v>42846</v>
@@ -730,10 +724,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="1">
         <v>42846</v>
@@ -753,7 +747,7 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F4" s="1">
         <v>42846</v>
@@ -770,10 +764,10 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" s="1">
         <v>42846</v>
@@ -793,7 +787,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" s="1">
         <v>42846</v>
@@ -810,10 +804,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" s="1">
         <v>42846</v>
@@ -830,10 +824,10 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F8" s="1">
         <v>42846</v>
@@ -850,10 +844,10 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" s="1">
         <v>42846</v>
@@ -870,10 +864,10 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" s="1">
         <v>42846</v>
@@ -890,10 +884,10 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" s="1">
         <v>42846</v>
@@ -913,7 +907,7 @@
         <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="1">
         <v>42846</v>
@@ -930,10 +924,10 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1">
         <v>42846</v>
@@ -950,10 +944,10 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14" s="1">
         <v>42846</v>
@@ -970,10 +964,10 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" s="1">
         <v>42846</v>
@@ -990,10 +984,10 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" s="1">
         <v>42846</v>
@@ -1010,10 +1004,10 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17" s="1">
         <v>42846</v>
@@ -1033,7 +1027,7 @@
         <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="1">
         <v>42846</v>
@@ -1050,10 +1044,10 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F19" s="1">
         <v>42846</v>
@@ -1073,7 +1067,7 @@
         <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F20" s="1">
         <v>42846</v>
@@ -1093,7 +1087,7 @@
         <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F21" s="1">
         <v>42846</v>
@@ -1110,13 +1104,13 @@
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F22" s="1">
-        <v>42846</v>
+        <v>42871</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1130,13 +1124,13 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F23" s="1">
-        <v>42846</v>
+        <v>42871</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1150,10 +1144,10 @@
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F24" s="1">
         <v>42846</v>
@@ -1170,10 +1164,10 @@
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F25" s="1">
         <v>42846</v>
@@ -1190,10 +1184,10 @@
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F26" s="1">
         <v>42846</v>
@@ -1210,10 +1204,10 @@
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F27" s="1">
         <v>42846</v>
@@ -1230,13 +1224,13 @@
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="E28" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F28" s="1">
-        <v>42846</v>
+        <v>42871</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1244,16 +1238,16 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F29" s="1">
         <v>42846</v>
@@ -1264,16 +1258,16 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F30" s="1">
         <v>42846</v>
@@ -1284,16 +1278,16 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F31" s="1">
         <v>42846</v>
@@ -1304,16 +1298,16 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F32" s="1">
         <v>42846</v>
@@ -1324,16 +1318,16 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F33" s="1">
         <v>42846</v>
@@ -1344,16 +1338,16 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F34" s="1">
         <v>42846</v>
@@ -1364,16 +1358,16 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F35" s="1">
         <v>42846</v>
@@ -1384,16 +1378,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F36" s="1">
         <v>42846</v>
@@ -1404,19 +1398,19 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="E37" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F37" s="1">
-        <v>42846</v>
+        <v>42871</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1424,16 +1418,16 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" t="s">
         <v>51</v>
-      </c>
-      <c r="C38" t="s">
-        <v>52</v>
       </c>
       <c r="D38" t="s">
         <v>34</v>
       </c>
       <c r="E38" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F38" s="1">
         <v>42846</v>
@@ -1444,16 +1438,16 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F39" s="1">
         <v>42846</v>
@@ -1464,16 +1458,16 @@
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F40" s="1">
         <v>42846</v>
@@ -1484,16 +1478,16 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D41" t="s">
         <v>34</v>
       </c>
       <c r="E41" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F41" s="1">
         <v>42846</v>
@@ -1504,16 +1498,16 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F42" s="1">
         <v>42846</v>
@@ -1524,16 +1518,16 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F43" s="1">
         <v>42846</v>
@@ -1544,16 +1538,16 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F44" s="1">
         <v>42846</v>
@@ -1564,16 +1558,16 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F45" s="1">
         <v>42846</v>
@@ -1584,16 +1578,16 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F46" s="1">
         <v>42846</v>
@@ -1604,16 +1598,16 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
       </c>
       <c r="D47" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F47" s="1">
         <v>42846</v>
@@ -1624,16 +1618,16 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C48" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="E48" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F48" s="1">
         <v>42846</v>
@@ -1644,16 +1638,16 @@
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="E49" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F49" s="1">
         <v>42846</v>
@@ -1664,16 +1658,16 @@
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D50" t="s">
         <v>34</v>
       </c>
       <c r="E50" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F50" s="1">
         <v>42846</v>
@@ -1684,16 +1678,16 @@
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D51" t="s">
         <v>34</v>
       </c>
       <c r="E51" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F51" s="1">
         <v>42846</v>
@@ -1704,16 +1698,16 @@
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D52" t="s">
         <v>34</v>
       </c>
       <c r="E52" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F52" s="1">
         <v>42846</v>
@@ -1724,16 +1718,16 @@
         <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F53" s="1">
         <v>42846</v>
@@ -1744,16 +1738,16 @@
         <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D54" t="s">
         <v>34</v>
       </c>
       <c r="E54" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F54" s="1">
         <v>42846</v>
@@ -1764,16 +1758,16 @@
         <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D55" t="s">
         <v>34</v>
       </c>
       <c r="E55" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F55" s="1">
         <v>42846</v>
@@ -1784,16 +1778,16 @@
         <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D56" t="s">
         <v>34</v>
       </c>
       <c r="E56" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F56" s="1">
         <v>42846</v>
@@ -1801,19 +1795,19 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" t="s">
         <v>74</v>
       </c>
-      <c r="B57" t="s">
-        <v>75</v>
-      </c>
       <c r="C57" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="E57" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F57" s="1">
         <v>42846</v>
@@ -1821,19 +1815,19 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
       </c>
       <c r="D58" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F58" s="1">
         <v>42846</v>
@@ -1841,19 +1835,19 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C59" t="s">
         <v>6</v>
       </c>
       <c r="D59" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F59" s="1">
         <v>42846</v>
@@ -1861,19 +1855,19 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B60" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F60" s="1">
         <v>42846</v>
@@ -1881,19 +1875,19 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B61" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="D61" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="E61" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="F61" s="1">
         <v>42846</v>
@@ -1901,19 +1895,19 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B62" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C62" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D62" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="E62" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F62" s="1">
         <v>42846</v>
@@ -1921,19 +1915,19 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B63" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
       </c>
       <c r="D63" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F63" s="1">
         <v>42846</v>
@@ -1941,7 +1935,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B64" t="s">
         <v>83</v>
@@ -1950,10 +1944,10 @@
         <v>6</v>
       </c>
       <c r="D64" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F64" s="1">
         <v>42846</v>
@@ -1961,19 +1955,19 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B65" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E65" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F65" s="1">
         <v>42846</v>
@@ -1981,19 +1975,19 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B66" t="s">
+        <v>86</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" t="s">
         <v>87</v>
       </c>
-      <c r="C66" t="s">
-        <v>6</v>
-      </c>
-      <c r="D66" t="s">
-        <v>97</v>
-      </c>
       <c r="E66" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="F66" s="1">
         <v>42846</v>
@@ -2001,19 +1995,19 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67" t="s">
         <v>88</v>
       </c>
-      <c r="B67" t="s">
-        <v>89</v>
-      </c>
       <c r="C67" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="D67" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="E67" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F67" s="1">
         <v>42846</v>
@@ -2021,93 +2015,73 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B68" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C68" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D68" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="E68" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F68" s="1">
         <v>42846</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>88</v>
-      </c>
-      <c r="B69" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B70" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C69" t="s">
-        <v>6</v>
-      </c>
-      <c r="D69" t="s">
-        <v>93</v>
-      </c>
-      <c r="E69" t="s">
-        <v>85</v>
-      </c>
-      <c r="F69" s="1">
-        <v>42846</v>
+      <c r="C70" s="2">
+        <f>COUNTA(C2:C68)</f>
+        <v>67</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E70" s="2">
+        <f>COUNTA(E2:E68)</f>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B71" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C71" s="2">
-        <f>COUNTA(C2:C69)</f>
-        <v>68</v>
+        <f>COUNTIF(C2:C68,"=YES")</f>
+        <v>57</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E71" s="2">
-        <f>COUNTA(E2:E69)</f>
-        <v>68</v>
+        <f>COUNTIF(E2:E68,"=YES")</f>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B72" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C72" s="2">
-        <f>COUNTIF(C2:C69,"=YES")</f>
-        <v>55</v>
+        <f>C71/C70*100</f>
+        <v>85.074626865671647</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E72" s="2">
-        <f>COUNTIF(E2:E69,"=YES")</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B73" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C73" s="2">
-        <f>C72/C71*100</f>
-        <v>80.882352941176478</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E73" s="2">
-        <f>100-E72/E71*100</f>
-        <v>67.64705882352942</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>96</v>
+        <f>100-E71/E70*100</f>
+        <v>74.626865671641795</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>